<commit_message>
updated xlsx file with comments
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/NRGI-RGI/NRGI-RGI.xlsx
+++ b/Simple_XLS_Importer/data/NRGI-RGI/NRGI-RGI.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
   <si>
     <t>Algeria</t>
   </si>
@@ -357,6 +357,18 @@
   </si>
   <si>
     <t>RGI-MINING</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>(Alberta)</t>
+  </si>
+  <si>
+    <t>(Gulf of Mexico)</t>
+  </si>
+  <si>
+    <t>(Western)</t>
   </si>
 </sst>
 </file>
@@ -753,7 +765,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -774,7 +786,9 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -832,6 +846,9 @@
       <c r="D5">
         <v>75</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -845,6 +862,9 @@
       </c>
       <c r="D6">
         <v>74</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -887,6 +907,9 @@
       </c>
       <c r="D9">
         <v>71</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>